<commit_message>
Updated ip in excel
</commit_message>
<xml_diff>
--- a/resources/datarepo/urls.xlsx
+++ b/resources/datarepo/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\NextGen Cloudlabs\Presentation\Free Labs Session\DevOps-CICD-Automation-Demo\resources\datarepo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65F185B-425D-4A5D-BA23-5AA8FCB47799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048111FA-C9D5-4B6D-BA37-904898211F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>prod-links</t>
   </si>
   <si>
-    <t>http://172.31.15.230:8083</t>
+    <t>http://172.31.23.107:8082/webapp/</t>
   </si>
   <si>
-    <t>http://172.31.15.230:8082/webapp/</t>
+    <t>http://172.31.23.107:8083</t>
+  </si>
+  <si>
+    <t>http://172.31.29.70:8082/webapp</t>
+  </si>
+  <si>
+    <t>http://172.31.29.70:8083</t>
   </si>
 </sst>
 </file>
@@ -362,7 +368,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A50575F-F4D8-4FA7-A672-9105584A5E0F}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -378,18 +384,30 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{39942109-3D18-4B3A-834E-94C734531C5E}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{C555BBFE-C35F-439C-8150-F292F6655669}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{23F9916A-00D0-430F-9DEF-D5B7F99AAC7B}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{9316A1DD-E2F2-45B1-A0C2-40BFCE58482C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>